<commit_message>
update the data, lack dali and baselie, rerun dali
</commit_message>
<xml_diff>
--- a/cifar.xlsx
+++ b/cifar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\yh\INR_draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F75A086-C534-4345-8CA1-70B62588FAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B6BF4C-6D0A-413E-AE76-D6325E51B9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37815" yWindow="3420" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,13 +527,11 @@
         <v>4</v>
       </c>
       <c r="B2" s="5">
-        <v>250</v>
-      </c>
-      <c r="C2" s="3">
-        <v>120</v>
-      </c>
+        <v>253.3</v>
+      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -541,13 +539,11 @@
         <v>5</v>
       </c>
       <c r="B3" s="5">
-        <v>131</v>
-      </c>
-      <c r="C3" s="3">
-        <v>117</v>
-      </c>
+        <v>132.5</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,13 +551,11 @@
         <v>6</v>
       </c>
       <c r="B4" s="5">
-        <v>120</v>
-      </c>
-      <c r="C4" s="3">
-        <v>116</v>
-      </c>
+        <v>126.3</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -569,13 +563,11 @@
         <v>7</v>
       </c>
       <c r="B5" s="5">
-        <v>120</v>
-      </c>
-      <c r="C5" s="3">
-        <v>116</v>
-      </c>
+        <v>128.19999999999999</v>
+      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,13 +575,11 @@
         <v>8</v>
       </c>
       <c r="B6" s="5">
-        <v>122</v>
-      </c>
-      <c r="C6" s="3">
-        <v>119</v>
-      </c>
+        <v>127.4</v>
+      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,13 +587,11 @@
         <v>9</v>
       </c>
       <c r="B7" s="5">
-        <v>122</v>
-      </c>
-      <c r="C7" s="3">
-        <v>115</v>
-      </c>
+        <v>128.19999999999999</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,13 +599,11 @@
         <v>10</v>
       </c>
       <c r="B8" s="5">
-        <v>121</v>
-      </c>
-      <c r="C8" s="3">
-        <v>116</v>
-      </c>
+        <v>128.5</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,13 +611,11 @@
         <v>11</v>
       </c>
       <c r="B9" s="5">
-        <v>128</v>
-      </c>
-      <c r="C9" s="3">
-        <v>119</v>
-      </c>
+        <v>129.30000000000001</v>
+      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="6">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>